<commit_message>
Updated info, updated N22
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Gadgets\Philips PM2528 DMM\Schematics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Gadgets\Philips PM2528 DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3386CE94-8998-4FE6-9559-8FCAD824039A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409ED6A8-00F8-4911-9B07-C9018EF8FCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-390" yWindow="3705" windowWidth="29970" windowHeight="17340" activeTab="1" xr2:uid="{1BACE0FD-08C6-41B4-8CD8-ADA47AB22099}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{1BACE0FD-08C6-41B4-8CD8-ADA47AB22099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="N23-Ranges" sheetId="2" r:id="rId2"/>
+    <sheet name="MainBoard-Relais" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="122">
   <si>
     <t>Pin</t>
   </si>
@@ -385,13 +386,31 @@
   </si>
   <si>
     <t>1pA</t>
+  </si>
+  <si>
+    <t>200mV</t>
+  </si>
+  <si>
+    <t>2V</t>
+  </si>
+  <si>
+    <t>20V</t>
+  </si>
+  <si>
+    <t>200V</t>
+  </si>
+  <si>
+    <t>2000V</t>
+  </si>
+  <si>
+    <t>VDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +435,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -448,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -468,6 +495,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1584,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C98CD3F-5F74-4E13-AD64-0C1C70D014E9}">
   <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,28 +1946,28 @@
       <c r="B14" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1951,19 +1984,19 @@
       <c r="E15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="7" t="s">
+      <c r="F15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>96</v>
       </c>
       <c r="K15" s="7"/>
@@ -1974,4 +2007,288 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13E4AE5-51C0-4E59-B711-92BE55C33E5F}">
+  <dimension ref="A2:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3">
+        <v>1202</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3">
+        <v>1203</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3">
+        <v>1204</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3">
+        <v>1301</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3">
+        <v>1302</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3">
+        <v>1303</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3">
+        <v>1306</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3">
+        <v>1609</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>